<commit_message>
fixed weak scaling plots
</commit_message>
<xml_diff>
--- a/projects/02-OpenMP/01-report/charts.xlsx
+++ b/projects/02-OpenMP/01-report/charts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="strong" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="26">
   <si>
     <t>Threads</t>
   </si>
@@ -204,10 +204,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -662,11 +662,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1635530144"/>
-        <c:axId val="1660714560"/>
+        <c:axId val="-358214336"/>
+        <c:axId val="-358916176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1635530144"/>
+        <c:axId val="-358214336"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -780,12 +780,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1660714560"/>
+        <c:crossAx val="-358916176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1660714560"/>
+        <c:axId val="-358916176"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -898,7 +898,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1635530144"/>
+        <c:crossAx val="-358214336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1407,11 +1407,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1727874432"/>
-        <c:axId val="1722438512"/>
+        <c:axId val="-358187600"/>
+        <c:axId val="-358183328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1727874432"/>
+        <c:axId val="-358187600"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1525,12 +1525,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1722438512"/>
+        <c:crossAx val="-358183328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1722438512"/>
+        <c:axId val="-358183328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1644,7 +1644,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1727874432"/>
+        <c:crossAx val="-358187600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="0.02"/>
@@ -2460,11 +2460,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1594659504"/>
-        <c:axId val="1656330960"/>
+        <c:axId val="-395800176"/>
+        <c:axId val="-395790064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1594659504"/>
+        <c:axId val="-395800176"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2541,6 +2541,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2577,12 +2578,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1656330960"/>
+        <c:crossAx val="-395790064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1656330960"/>
+        <c:axId val="-395790064"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2695,7 +2696,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1594659504"/>
+        <c:crossAx val="-395800176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3510,11 +3511,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1724212704"/>
-        <c:axId val="1724777200"/>
+        <c:axId val="-358132768"/>
+        <c:axId val="-358129008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1724212704"/>
+        <c:axId val="-358132768"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -3627,12 +3628,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1724777200"/>
+        <c:crossAx val="-358129008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1724777200"/>
+        <c:axId val="-358129008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3744,7 +3745,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1724212704"/>
+        <c:crossAx val="-358132768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3788,6 +3789,779 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>weak!$Q$49:$Q$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1414.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2828.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5657.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>weak!$R$49:$R$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.906326916125923</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.693404348899685</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.272478510195298</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.292437232598</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.0551910918776</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00">
+                  <c:v>50.12791049574771</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-262860288"/>
+        <c:axId val="-262857808"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-262860288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Particles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-262857808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-262857808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Efficiency (T1/Tp)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-262860288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>weak!$Q$15:$Q$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1414.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2828.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5657.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>weak!$R$15:$R$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.609648</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.788752</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.757893</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.751072</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.822763</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.839027</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.178754</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-263737008"/>
+        <c:axId val="-263419664"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-263737008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Particles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-263419664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-263419664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3.4"/>
+          <c:min val="2.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Speed-Up</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-263737008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3985,6 +4759,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6030,6 +6884,1012 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6123,13 +7983,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6154,13 +8014,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6177,6 +8037,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>374650</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>374650</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6450,7 +8370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -6609,7 +8529,7 @@
         <v>0.76727299999999998</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C3:C5" si="5">B$2/B4</f>
+        <f t="shared" ref="C4:C5" si="5">B$2/B4</f>
         <v>3.5183656925240427</v>
       </c>
       <c r="D4" s="2">
@@ -6711,7 +8631,7 @@
         <v>7.9200904802140544</v>
       </c>
       <c r="D6" s="2">
-        <f t="shared" ref="D3:D7" si="7">C6/$A6</f>
+        <f t="shared" ref="D6:D7" si="7">C6/$A6</f>
         <v>0.4950056550133784</v>
       </c>
       <c r="E6">
@@ -6866,10 +8786,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:V82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:V8"/>
+    <sheetView tabSelected="1" topLeftCell="P38" workbookViewId="0">
+      <selection activeCell="W44" sqref="W44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6887,6 +8807,7 @@
     <col min="12" max="12" width="7" customWidth="1"/>
     <col min="13" max="13" width="6.83203125" customWidth="1"/>
     <col min="14" max="14" width="14.1640625" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -6920,40 +8841,40 @@
       <c r="J1" s="5">
         <v>2000</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="8">
+      <c r="L1" s="7">
         <v>2828</v>
       </c>
-      <c r="M1" s="8">
+      <c r="M1" s="7">
         <v>2828</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="8">
+      <c r="O1" s="7">
         <v>4000</v>
       </c>
-      <c r="P1" s="8">
+      <c r="P1" s="7">
         <v>4000</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="8">
+      <c r="R1" s="7">
         <v>5657</v>
       </c>
-      <c r="S1" s="8">
+      <c r="S1" s="7">
         <v>5657</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="8">
+      <c r="U1" s="7">
         <v>8000</v>
       </c>
-      <c r="V1" s="8">
+      <c r="V1" s="7">
         <v>8000</v>
       </c>
     </row>
@@ -7531,8 +9452,180 @@
         <v>0.78324860149605791</v>
       </c>
     </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Q15" s="5">
+        <v>1000</v>
+      </c>
+      <c r="R15">
+        <v>2.609648</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Q16" s="5">
+        <v>1414</v>
+      </c>
+      <c r="R16">
+        <v>2.7887520000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q17" s="5">
+        <v>2000</v>
+      </c>
+      <c r="R17">
+        <v>2.7578930000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q18" s="7">
+        <v>2828</v>
+      </c>
+      <c r="R18">
+        <v>2.7510720000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q19" s="7">
+        <v>4000</v>
+      </c>
+      <c r="R19">
+        <v>2.8227630000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q20" s="7">
+        <v>5657</v>
+      </c>
+      <c r="R20">
+        <v>2.8390270000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q21" s="7">
+        <v>8000</v>
+      </c>
+      <c r="R21">
+        <v>3.1787540000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q49" s="5">
+        <v>1000</v>
+      </c>
+      <c r="R49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q50" s="5">
+        <v>1414</v>
+      </c>
+      <c r="R50">
+        <v>1.9063269161259229</v>
+      </c>
+    </row>
+    <row r="51" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q51" s="5">
+        <v>2000</v>
+      </c>
+      <c r="R51">
+        <v>3.6934043488996853</v>
+      </c>
+    </row>
+    <row r="52" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q52" s="7">
+        <v>2828</v>
+      </c>
+      <c r="R52">
+        <v>7.272478510195298</v>
+      </c>
+    </row>
+    <row r="53" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q53" s="7">
+        <v>4000</v>
+      </c>
+      <c r="R53">
+        <v>14.29243723259799</v>
+      </c>
+    </row>
+    <row r="54" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q54" s="7">
+        <v>5657</v>
+      </c>
+      <c r="R54">
+        <v>27.055191091877603</v>
+      </c>
+    </row>
+    <row r="55" spans="17:18" x14ac:dyDescent="0.2">
+      <c r="Q55" s="7">
+        <v>8000</v>
+      </c>
+      <c r="R55" s="1">
+        <v>50.127910495747706</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R74" s="6"/>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A76" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76">
+        <v>2.609648</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A77" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B77">
+        <v>2.7887520000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78">
+        <v>2.7578930000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A79" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79">
+        <v>2.7510720000000002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A80" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B80">
+        <v>2.8227630000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81">
+        <v>2.8390270000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B82">
+        <v>3.1787540000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -7541,7 +9634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -7556,14 +9649,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="H1" s="7" t="s">
+      <c r="C1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="7"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -7602,10 +9695,10 @@
       <c r="O2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">

</xml_diff>